<commit_message>
Moved Map to server, added printing functions for players once i make sprites
</commit_message>
<xml_diff>
--- a/checkmap.xlsx
+++ b/checkmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nepplnj\Documents\GitHub\testing-dnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEED1ED-933F-426A-BF83-81C29C7C0B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457E3725-DBC6-41B9-9EAC-B755C8E48355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1710" windowWidth="10860" windowHeight="11260" xr2:uid="{C5A0DFAB-F768-4A8D-AC68-42063D2970FE}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="9330" windowHeight="11260" xr2:uid="{C5A0DFAB-F768-4A8D-AC68-42063D2970FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,59 +405,59 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>2</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -469,949 +465,949 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
         <v>2</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P17">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>